<commit_message>
new file:   Documents/presentation doc/App Structure.pptx 	modified:   Documents/proposal/Project plan.xlsx 	new file:   Documents/weekly report/JongUk Kim/Weekly report_JongUk-Kim_20120329.docx 	new file:   Documents/weekly report/Sanghyun Lee/Weekly report_SangHyun-Lee_20120329.docx 	new file:   Documents/weekly report/Team/Weekly report_Lemonade_20120329.docx 	new file:   Documents/weekly report/YoonJae Lee/Weekly report_YoonJae-Lee_20120329.docx
</commit_message>
<xml_diff>
--- a/Documents/proposal/Project plan.xlsx
+++ b/Documents/proposal/Project plan.xlsx
@@ -11,12 +11,15 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$S$37</definedName>
+  </definedNames>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="59">
   <si>
     <t>주제 선정</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -66,10 +69,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>구현</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>설계</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -82,15 +81,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Android &amp; JNI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>팀</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>USB/IP 포팅</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -123,24 +114,36 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Android App</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Service
-App</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Android-USB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>USB드라이버</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Android App</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VHCI 드라이버</t>
+(터치마우스)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Device Driver</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USB/IP로 변경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Device Driver</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>터치서비스 부분</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -148,14 +151,54 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>USB/IP Porting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VHCI Driver</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stub_driver.c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bind-driver.c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Usbip_network.c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>??</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ProtoType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중간1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중간2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최종</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>윤재</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>인구</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>상현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -164,19 +207,56 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>팀</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>인구</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상현, 윤재</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>인구, 종욱</t>
+    <t>USB/IP 연결 부분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Android 크로스 컴파일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>커널 Configuration</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JNI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Android 구조</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Windows App (Play)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Windows App (Recv)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Windows App (Send)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Windows App (Text Input)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Android App (Send)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Android App (Recv)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Android App (Capture)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Service
+(카카오톡 연동)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -184,7 +264,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,17 +316,8 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0" tint="-0.34998626667073579"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="11">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -279,12 +350,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -295,20 +360,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF79646"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="16">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -527,13 +580,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -552,116 +655,131 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -671,10 +789,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF3AA2F8"/>
       <color rgb="FF7FFE4C"/>
       <color rgb="FFF79646"/>
       <color rgb="FF7030A0"/>
-      <color rgb="FF3AA2F8"/>
       <color rgb="FF3232FF"/>
       <color rgb="FF0000FF"/>
     </mruColors>
@@ -974,57 +1092,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:S21"/>
+  <dimension ref="B1:W40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10.375" customWidth="1"/>
     <col min="3" max="3" width="8.625" customWidth="1"/>
-    <col min="4" max="4" width="13.875" customWidth="1"/>
+    <col min="4" max="4" width="28.75" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="19" width="4" customWidth="1"/>
+    <col min="20" max="20" width="3.125" customWidth="1"/>
+    <col min="22" max="22" width="5.75" customWidth="1"/>
+    <col min="23" max="23" width="2.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B2" s="26"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22" t="s">
+    <row r="1" spans="2:23" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="39"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21" t="s">
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21" t="s">
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21" t="s">
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="22"/>
-    </row>
-    <row r="3" spans="2:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B3" s="23"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25"/>
+      <c r="S2" s="37"/>
+    </row>
+    <row r="3" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="29"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="38"/>
       <c r="F3" s="1">
         <v>1</v>
       </c>
@@ -1068,14 +1189,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B4" s="23" t="s">
+    <row r="4" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
       <c r="E4" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="2"/>
@@ -1092,16 +1213,16 @@
       <c r="R4" s="2"/>
       <c r="S4" s="3"/>
     </row>
-    <row r="5" spans="2:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B5" s="23" t="s">
+    <row r="5" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="24"/>
+      <c r="D5" s="30"/>
       <c r="E5" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="5"/>
@@ -1118,19 +1239,19 @@
       <c r="R5" s="2"/>
       <c r="S5" s="3"/>
     </row>
-    <row r="6" spans="2:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B6" s="23"/>
-      <c r="C6" s="24" t="s">
+    <row r="6" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="29"/>
+      <c r="C6" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="24"/>
+      <c r="D6" s="30"/>
       <c r="E6" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="39"/>
+      <c r="I6" s="16"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -1142,14 +1263,14 @@
       <c r="R6" s="2"/>
       <c r="S6" s="3"/>
     </row>
-    <row r="7" spans="2:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B7" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="24" t="s">
+    <row r="7" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="24"/>
+      <c r="D7" s="30"/>
       <c r="E7" s="3" t="s">
         <v>10</v>
       </c>
@@ -1167,21 +1288,29 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="3"/>
-    </row>
-    <row r="8" spans="2:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B8" s="23"/>
-      <c r="C8" s="24" t="s">
+      <c r="U7" s="18"/>
+      <c r="V7" t="s">
+        <v>44</v>
+      </c>
+      <c r="W7">
+        <f>COUNTIF($E$15:$E$34,V7)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="34"/>
+      <c r="C8" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="24"/>
+      <c r="D8" s="30"/>
       <c r="E8" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
+        <v>10</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -1191,20 +1320,28 @@
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
       <c r="S8" s="3"/>
-    </row>
-    <row r="9" spans="2:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B9" s="23"/>
-      <c r="C9" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="24"/>
+      <c r="U8" s="19"/>
+      <c r="V8" t="s">
+        <v>42</v>
+      </c>
+      <c r="W8">
+        <f>COUNTIF($E$15:$E$34,V8)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="34"/>
+      <c r="C9" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="30"/>
       <c r="E9" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
+        <v>10</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -1215,101 +1352,108 @@
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
       <c r="S9" s="3"/>
-    </row>
-    <row r="10" spans="2:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B10" s="23" t="s">
+      <c r="U9" s="15"/>
+      <c r="V9" t="s">
+        <v>45</v>
+      </c>
+      <c r="W9">
+        <f>COUNTIF($E$15:$E$34,V9)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="34"/>
+      <c r="C10" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="32"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="21"/>
+      <c r="U10" s="14"/>
+      <c r="V10" t="s">
+        <v>43</v>
+      </c>
+      <c r="W10">
+        <f>COUNTIF($E$15:$E$34,V10)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="34"/>
+      <c r="C11" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="32"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="21"/>
+    </row>
+    <row r="12" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="35"/>
+      <c r="C12" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="32"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="21"/>
+    </row>
+    <row r="13" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="3"/>
-    </row>
-    <row r="11" spans="2:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B11" s="23"/>
-      <c r="C11" s="24" t="s">
+      <c r="D13" s="30"/>
+      <c r="E13" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="3"/>
-    </row>
-    <row r="12" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="3"/>
-    </row>
-    <row r="13" spans="2:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B13" s="23"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
@@ -1317,229 +1461,668 @@
       <c r="R13" s="2"/>
       <c r="S13" s="3"/>
     </row>
-    <row r="14" spans="2:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B14" s="23"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="11" t="s">
+    <row r="14" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="29"/>
+      <c r="C14" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="30"/>
+      <c r="E14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="3"/>
+    </row>
+    <row r="15" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="45"/>
+      <c r="C15" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="26"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="24"/>
+      <c r="R15" s="24"/>
+      <c r="S15" s="25"/>
+    </row>
+    <row r="16" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="45"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="26"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="24"/>
+      <c r="S16" s="25"/>
+    </row>
+    <row r="17" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="45"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="26"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="24"/>
+      <c r="S17" s="25"/>
+    </row>
+    <row r="18" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="45"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="26"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="24"/>
+      <c r="S18" s="25"/>
+    </row>
+    <row r="19" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="45"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="26"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="24"/>
+      <c r="S19" s="25"/>
+    </row>
+    <row r="20" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="45"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="26"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="24"/>
+      <c r="S20" s="25"/>
+    </row>
+    <row r="21" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="45"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="3"/>
+    </row>
+    <row r="22" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="45"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="13"/>
+    </row>
+    <row r="23" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="45"/>
+      <c r="C23" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="3"/>
+    </row>
+    <row r="24" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="45"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="12"/>
+      <c r="S24" s="13"/>
+    </row>
+    <row r="25" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="45"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="13"/>
+    </row>
+    <row r="26" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="45"/>
+      <c r="C26" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E26" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="14"/>
+      <c r="Q26" s="14"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="13"/>
+    </row>
+    <row r="27" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="45"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" s="26"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="17"/>
+      <c r="R27" s="24"/>
+      <c r="S27" s="25"/>
+    </row>
+    <row r="28" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="45"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="17"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="3"/>
+    </row>
+    <row r="29" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="45"/>
+      <c r="C29" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="26"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="24"/>
+      <c r="P29" s="24"/>
+      <c r="Q29" s="24"/>
+      <c r="R29" s="24"/>
+      <c r="S29" s="25"/>
+    </row>
+    <row r="30" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="45"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" s="26"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="24"/>
+      <c r="P30" s="24"/>
+      <c r="Q30" s="24"/>
+      <c r="R30" s="24"/>
+      <c r="S30" s="25"/>
+    </row>
+    <row r="31" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="45"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="26"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="24"/>
+      <c r="Q31" s="24"/>
+      <c r="R31" s="24"/>
+      <c r="S31" s="25"/>
+    </row>
+    <row r="32" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="45"/>
+      <c r="C32" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="18"/>
-    </row>
-    <row r="15" spans="2:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B15" s="23"/>
-      <c r="C15" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="11" t="s">
+      <c r="E32" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F32" s="26"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="24"/>
+      <c r="Q32" s="24"/>
+      <c r="R32" s="24"/>
+      <c r="S32" s="25"/>
+    </row>
+    <row r="33" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="46"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F33" s="26"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="24"/>
+      <c r="Q33" s="24"/>
+      <c r="R33" s="24"/>
+      <c r="S33" s="25"/>
+    </row>
+    <row r="34" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="36"/>
-      <c r="O15" s="36"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="3"/>
-    </row>
-    <row r="16" spans="2:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B16" s="23"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="40"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="39"/>
-      <c r="O16" s="39"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="3"/>
-    </row>
-    <row r="17" spans="2:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B17" s="23"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="38"/>
-      <c r="O17" s="38"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="3"/>
-    </row>
-    <row r="18" spans="2:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B18" s="23" t="s">
+      <c r="D34" s="7"/>
+      <c r="E34" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="26"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="24"/>
+      <c r="R34" s="24"/>
+      <c r="S34" s="25"/>
+    </row>
+    <row r="35" spans="2:19" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B35" s="29"/>
+      <c r="C35" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="24"/>
+      <c r="E35" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="26"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="24"/>
+      <c r="K35" s="24"/>
+      <c r="L35" s="24"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5"/>
+      <c r="R35" s="24"/>
+      <c r="S35" s="25"/>
+    </row>
+    <row r="36" spans="2:19" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B36" s="29"/>
+      <c r="C36" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="D36" s="24"/>
+      <c r="E36" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="26"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="24"/>
+      <c r="K36" s="24"/>
+      <c r="L36" s="24"/>
+      <c r="M36" s="24"/>
+      <c r="N36" s="24"/>
+      <c r="O36" s="24"/>
+      <c r="P36" s="24"/>
+      <c r="Q36" s="5"/>
+      <c r="R36" s="5"/>
+      <c r="S36" s="25"/>
+    </row>
+    <row r="37" spans="2:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="3"/>
-    </row>
-    <row r="19" spans="2:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B19" s="23"/>
-      <c r="C19" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="3"/>
-    </row>
-    <row r="20" spans="2:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B20" s="23"/>
-      <c r="C20" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="3"/>
-    </row>
-    <row r="21" spans="2:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="14"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
-      <c r="S21" s="16"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="9"/>
+      <c r="O37" s="9"/>
+      <c r="P37" s="9"/>
+      <c r="Q37" s="9"/>
+      <c r="R37" s="9"/>
+      <c r="S37" s="10"/>
+    </row>
+    <row r="38" spans="2:19" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D38" s="47"/>
+      <c r="E38" s="47"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="47"/>
+      <c r="H38" s="47"/>
+      <c r="I38" s="47"/>
+      <c r="J38" s="47"/>
+      <c r="K38" s="47"/>
+      <c r="L38" s="47"/>
+      <c r="M38" s="47"/>
+      <c r="N38" s="47"/>
+      <c r="O38" s="47"/>
+      <c r="P38" s="47"/>
+      <c r="Q38" s="47"/>
+      <c r="R38" s="47"/>
+      <c r="S38" s="47"/>
+    </row>
+    <row r="40" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="K40" t="s">
+        <v>38</v>
+      </c>
+      <c r="O40" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>40</v>
+      </c>
+      <c r="S40" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B17"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="F2:I2"/>
+  <autoFilter ref="B2:S37">
+    <filterColumn colId="0" showButton="0"/>
+    <filterColumn colId="1" showButton="0"/>
+    <filterColumn colId="4" showButton="0"/>
+    <filterColumn colId="5" showButton="0"/>
+    <filterColumn colId="6" showButton="0"/>
+    <filterColumn colId="8" showButton="0"/>
+    <filterColumn colId="9" showButton="0"/>
+    <filterColumn colId="10" showButton="0"/>
+    <filterColumn colId="12" showButton="0"/>
+    <filterColumn colId="13" showButton="0"/>
+    <filterColumn colId="14" showButton="0"/>
+    <filterColumn colId="16" showButton="0"/>
+  </autoFilter>
+  <mergeCells count="27">
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="B15:B33"/>
+    <mergeCell ref="C15:C22"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:S2"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="B2:D3"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="B7:B12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
modified:   Documents/presentation doc/App Structure.pptx 	modified:   Documents/proposal/Project plan.xlsx
</commit_message>
<xml_diff>
--- a/Documents/proposal/Project plan.xlsx
+++ b/Documents/proposal/Project plan.xlsx
@@ -636,7 +636,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -724,10 +724,49 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -744,42 +783,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1095,7 +1098,7 @@
   <dimension ref="B1:W40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="Z20" sqref="Z20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1112,40 +1115,40 @@
   <sheetData>
     <row r="1" spans="2:23" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="39"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="37" t="s">
+      <c r="B2" s="42"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36" t="s">
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36" t="s">
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36" t="s">
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="S2" s="37"/>
+      <c r="S2" s="39"/>
     </row>
     <row r="3" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="29"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="38"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="41"/>
       <c r="F3" s="1">
         <v>1</v>
       </c>
@@ -1190,11 +1193,11 @@
       </c>
     </row>
     <row r="4" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="3" t="s">
         <v>15</v>
       </c>
@@ -1214,13 +1217,13 @@
       <c r="S4" s="3"/>
     </row>
     <row r="5" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="30"/>
+      <c r="D5" s="40"/>
       <c r="E5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1240,11 +1243,11 @@
       <c r="S5" s="3"/>
     </row>
     <row r="6" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="29"/>
-      <c r="C6" s="30" t="s">
+      <c r="B6" s="34"/>
+      <c r="C6" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="30"/>
+      <c r="D6" s="40"/>
       <c r="E6" s="3" t="s">
         <v>15</v>
       </c>
@@ -1264,13 +1267,13 @@
       <c r="S6" s="3"/>
     </row>
     <row r="7" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="30"/>
+      <c r="D7" s="40"/>
       <c r="E7" s="3" t="s">
         <v>10</v>
       </c>
@@ -1298,11 +1301,11 @@
       </c>
     </row>
     <row r="8" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="34"/>
-      <c r="C8" s="30" t="s">
+      <c r="B8" s="47"/>
+      <c r="C8" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="30"/>
+      <c r="D8" s="40"/>
       <c r="E8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1330,11 +1333,11 @@
       </c>
     </row>
     <row r="9" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="34"/>
-      <c r="C9" s="30" t="s">
+      <c r="B9" s="47"/>
+      <c r="C9" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="30"/>
+      <c r="D9" s="40"/>
       <c r="E9" s="3" t="s">
         <v>10</v>
       </c>
@@ -1362,11 +1365,11 @@
       </c>
     </row>
     <row r="10" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="34"/>
-      <c r="C10" s="31" t="s">
+      <c r="B10" s="47"/>
+      <c r="C10" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="32"/>
+      <c r="D10" s="45"/>
       <c r="E10" s="21"/>
       <c r="F10" s="27"/>
       <c r="G10" s="6"/>
@@ -1392,11 +1395,11 @@
       </c>
     </row>
     <row r="11" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="34"/>
-      <c r="C11" s="31" t="s">
+      <c r="B11" s="47"/>
+      <c r="C11" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="32"/>
+      <c r="D11" s="45"/>
       <c r="E11" s="21"/>
       <c r="F11" s="27"/>
       <c r="G11" s="6"/>
@@ -1414,11 +1417,11 @@
       <c r="S11" s="21"/>
     </row>
     <row r="12" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="35"/>
-      <c r="C12" s="31" t="s">
+      <c r="B12" s="48"/>
+      <c r="C12" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="32"/>
+      <c r="D12" s="45"/>
       <c r="E12" s="21"/>
       <c r="F12" s="27"/>
       <c r="G12" s="6"/>
@@ -1436,13 +1439,13 @@
       <c r="S12" s="21"/>
     </row>
     <row r="13" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="30"/>
+      <c r="D13" s="40"/>
       <c r="E13" s="3" t="s">
         <v>15</v>
       </c>
@@ -1462,11 +1465,11 @@
       <c r="S13" s="3"/>
     </row>
     <row r="14" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="29"/>
-      <c r="C14" s="30" t="s">
+      <c r="B14" s="34"/>
+      <c r="C14" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="30"/>
+      <c r="D14" s="40"/>
       <c r="E14" s="3" t="s">
         <v>15</v>
       </c>
@@ -1486,8 +1489,8 @@
       <c r="S14" s="3"/>
     </row>
     <row r="15" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="45"/>
-      <c r="C15" s="42" t="s">
+      <c r="B15" s="36"/>
+      <c r="C15" s="32" t="s">
         <v>58</v>
       </c>
       <c r="D15" s="7" t="s">
@@ -1512,8 +1515,8 @@
       <c r="S15" s="25"/>
     </row>
     <row r="16" spans="2:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="45"/>
-      <c r="C16" s="42"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="32"/>
       <c r="D16" s="7" t="s">
         <v>52</v>
       </c>
@@ -1536,8 +1539,8 @@
       <c r="S16" s="25"/>
     </row>
     <row r="17" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="45"/>
-      <c r="C17" s="42"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="32"/>
       <c r="D17" s="7" t="s">
         <v>53</v>
       </c>
@@ -1560,8 +1563,8 @@
       <c r="S17" s="25"/>
     </row>
     <row r="18" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="45"/>
-      <c r="C18" s="42"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="32"/>
       <c r="D18" s="7" t="s">
         <v>54</v>
       </c>
@@ -1584,8 +1587,8 @@
       <c r="S18" s="25"/>
     </row>
     <row r="19" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="45"/>
-      <c r="C19" s="42"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="32"/>
       <c r="D19" s="7" t="s">
         <v>55</v>
       </c>
@@ -1596,9 +1599,9 @@
       <c r="G19" s="24"/>
       <c r="H19" s="24"/>
       <c r="I19" s="24"/>
-      <c r="J19" s="19"/>
+      <c r="J19" s="29"/>
       <c r="K19" s="19"/>
-      <c r="L19" s="11"/>
+      <c r="L19" s="19"/>
       <c r="M19" s="11"/>
       <c r="N19" s="24"/>
       <c r="O19" s="24"/>
@@ -1608,8 +1611,8 @@
       <c r="S19" s="25"/>
     </row>
     <row r="20" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="45"/>
-      <c r="C20" s="42"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="32"/>
       <c r="D20" s="7" t="s">
         <v>56</v>
       </c>
@@ -1620,9 +1623,9 @@
       <c r="G20" s="24"/>
       <c r="H20" s="24"/>
       <c r="I20" s="24"/>
-      <c r="J20" s="19"/>
+      <c r="J20" s="29"/>
       <c r="K20" s="19"/>
-      <c r="L20" s="11"/>
+      <c r="L20" s="19"/>
       <c r="M20" s="11"/>
       <c r="N20" s="24"/>
       <c r="O20" s="24"/>
@@ -1632,8 +1635,8 @@
       <c r="S20" s="25"/>
     </row>
     <row r="21" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="45"/>
-      <c r="C21" s="42"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="32"/>
       <c r="D21" s="7" t="s">
         <v>57</v>
       </c>
@@ -1656,8 +1659,8 @@
       <c r="S21" s="3"/>
     </row>
     <row r="22" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="45"/>
-      <c r="C22" s="43"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="33"/>
       <c r="D22" s="7" t="s">
         <v>28</v>
       </c>
@@ -1680,8 +1683,8 @@
       <c r="S22" s="13"/>
     </row>
     <row r="23" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="45"/>
-      <c r="C23" s="41" t="s">
+      <c r="B23" s="36"/>
+      <c r="C23" s="31" t="s">
         <v>26</v>
       </c>
       <c r="D23" s="7" t="s">
@@ -1706,8 +1709,8 @@
       <c r="S23" s="3"/>
     </row>
     <row r="24" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="45"/>
-      <c r="C24" s="42"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="32"/>
       <c r="D24" s="7" t="s">
         <v>30</v>
       </c>
@@ -1730,8 +1733,8 @@
       <c r="S24" s="13"/>
     </row>
     <row r="25" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="45"/>
-      <c r="C25" s="43"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="33"/>
       <c r="D25" s="7" t="s">
         <v>46</v>
       </c>
@@ -1754,8 +1757,8 @@
       <c r="S25" s="13"/>
     </row>
     <row r="26" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="45"/>
-      <c r="C26" s="41" t="s">
+      <c r="B26" s="36"/>
+      <c r="C26" s="31" t="s">
         <v>31</v>
       </c>
       <c r="D26" s="7" t="s">
@@ -1780,8 +1783,8 @@
       <c r="S26" s="13"/>
     </row>
     <row r="27" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="45"/>
-      <c r="C27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="32"/>
       <c r="D27" s="7" t="s">
         <v>16</v>
       </c>
@@ -1803,8 +1806,8 @@
       <c r="S27" s="25"/>
     </row>
     <row r="28" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="45"/>
-      <c r="C28" s="43"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="33"/>
       <c r="D28" s="7" t="s">
         <v>23</v>
       </c>
@@ -1827,8 +1830,8 @@
       <c r="S28" s="3"/>
     </row>
     <row r="29" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="45"/>
-      <c r="C29" s="44" t="s">
+      <c r="B29" s="36"/>
+      <c r="C29" s="35" t="s">
         <v>32</v>
       </c>
       <c r="D29" s="7" t="s">
@@ -1853,8 +1856,8 @@
       <c r="S29" s="25"/>
     </row>
     <row r="30" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="45"/>
-      <c r="C30" s="44"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="35"/>
       <c r="D30" s="7" t="s">
         <v>35</v>
       </c>
@@ -1877,8 +1880,8 @@
       <c r="S30" s="25"/>
     </row>
     <row r="31" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="45"/>
-      <c r="C31" s="44"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="35"/>
       <c r="D31" s="7" t="s">
         <v>36</v>
       </c>
@@ -1901,8 +1904,8 @@
       <c r="S31" s="25"/>
     </row>
     <row r="32" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="45"/>
-      <c r="C32" s="44" t="s">
+      <c r="B32" s="36"/>
+      <c r="C32" s="35" t="s">
         <v>33</v>
       </c>
       <c r="D32" s="7" t="s">
@@ -1927,8 +1930,8 @@
       <c r="S32" s="25"/>
     </row>
     <row r="33" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="46"/>
-      <c r="C33" s="44"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="35"/>
       <c r="D33" s="7" t="s">
         <v>37</v>
       </c>
@@ -1951,7 +1954,7 @@
       <c r="S33" s="25"/>
     </row>
     <row r="34" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="29" t="s">
+      <c r="B34" s="34" t="s">
         <v>17</v>
       </c>
       <c r="C34" s="24" t="s">
@@ -1977,7 +1980,7 @@
       <c r="S34" s="25"/>
     </row>
     <row r="35" spans="2:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B35" s="29"/>
+      <c r="B35" s="34"/>
       <c r="C35" s="24" t="s">
         <v>19</v>
       </c>
@@ -2001,7 +2004,7 @@
       <c r="S35" s="25"/>
     </row>
     <row r="36" spans="2:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B36" s="29"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="24" t="s">
         <v>20</v>
       </c>
@@ -2049,22 +2052,22 @@
       <c r="S37" s="10"/>
     </row>
     <row r="38" spans="2:19" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="D38" s="47"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="47"/>
-      <c r="H38" s="47"/>
-      <c r="I38" s="47"/>
-      <c r="J38" s="47"/>
-      <c r="K38" s="47"/>
-      <c r="L38" s="47"/>
-      <c r="M38" s="47"/>
-      <c r="N38" s="47"/>
-      <c r="O38" s="47"/>
-      <c r="P38" s="47"/>
-      <c r="Q38" s="47"/>
-      <c r="R38" s="47"/>
-      <c r="S38" s="47"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="30"/>
+      <c r="J38" s="30"/>
+      <c r="K38" s="30"/>
+      <c r="L38" s="30"/>
+      <c r="M38" s="30"/>
+      <c r="N38" s="30"/>
+      <c r="O38" s="30"/>
+      <c r="P38" s="30"/>
+      <c r="Q38" s="30"/>
+      <c r="R38" s="30"/>
+      <c r="S38" s="30"/>
     </row>
     <row r="40" spans="2:19" x14ac:dyDescent="0.3">
       <c r="K40" t="s">
@@ -2096,20 +2099,6 @@
     <filterColumn colId="16" showButton="0"/>
   </autoFilter>
   <mergeCells count="27">
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="B15:B33"/>
-    <mergeCell ref="C15:C22"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="B2:D3"/>
-    <mergeCell ref="F2:I2"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="C6:D6"/>
@@ -2123,6 +2112,20 @@
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="B7:B12"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="B2:D3"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="B15:B33"/>
+    <mergeCell ref="C15:C22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new file:   Documents/weekly report/Team/Weekly report_Lemonade_20120503.docx
</commit_message>
<xml_diff>
--- a/Documents/proposal/Project plan.xlsx
+++ b/Documents/proposal/Project plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="30" windowWidth="20730" windowHeight="10020"/>
@@ -318,8 +318,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -758,7 +758,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -870,6 +870,72 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -903,77 +969,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1074,7 +1077,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1109,7 +1111,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1285,14 +1286,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:X45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="1.625" customWidth="1"/>
     <col min="2" max="2" width="10.375" customWidth="1"/>
@@ -1306,44 +1307,44 @@
     <col min="24" max="24" width="2.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="70"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="67" t="s">
+    <row r="1" spans="2:24" ht="12" customHeight="1" thickBot="1"/>
+    <row r="2" spans="2:24" ht="17.25" customHeight="1">
+      <c r="B2" s="49"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="71" t="s">
+      <c r="G2" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66" t="s">
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="66"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66" t="s">
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="66"/>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66" t="s">
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="T2" s="67"/>
-    </row>
-    <row r="3" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="48"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="69"/>
+      <c r="T2" s="45"/>
+    </row>
+    <row r="3" spans="2:24" ht="17.25" customHeight="1">
+      <c r="B3" s="46"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="48"/>
       <c r="G3" s="1">
         <v>1</v>
       </c>
@@ -1387,13 +1388,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="48" t="s">
+    <row r="4" spans="2:24" ht="17.25" customHeight="1">
+      <c r="B4" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
       <c r="F4" s="3" t="s">
         <v>15</v>
       </c>
@@ -1412,15 +1413,15 @@
       <c r="S4" s="2"/>
       <c r="T4" s="3"/>
     </row>
-    <row r="5" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="48" t="s">
+    <row r="5" spans="2:24" ht="17.25" customHeight="1">
+      <c r="B5" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
       <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1439,13 +1440,13 @@
       <c r="S5" s="2"/>
       <c r="T5" s="3"/>
     </row>
-    <row r="6" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="48"/>
-      <c r="C6" s="55" t="s">
+    <row r="6" spans="2:24" ht="17.25" customHeight="1">
+      <c r="B6" s="46"/>
+      <c r="C6" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
       <c r="F6" s="3" t="s">
         <v>15</v>
       </c>
@@ -1464,15 +1465,15 @@
       <c r="S6" s="2"/>
       <c r="T6" s="3"/>
     </row>
-    <row r="7" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="57" t="s">
+    <row r="7" spans="2:24" ht="17.25" customHeight="1">
+      <c r="B7" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
       <c r="F7" s="3" t="s">
         <v>10</v>
       </c>
@@ -1499,13 +1500,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="58"/>
-      <c r="C8" s="55" t="s">
+    <row r="8" spans="2:24" ht="17.25" customHeight="1">
+      <c r="B8" s="57"/>
+      <c r="C8" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
       <c r="F8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1532,13 +1533,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="58"/>
-      <c r="C9" s="55" t="s">
+    <row r="9" spans="2:24" ht="17.25" customHeight="1">
+      <c r="B9" s="57"/>
+      <c r="C9" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
       <c r="F9" s="3" t="s">
         <v>10</v>
       </c>
@@ -1565,13 +1566,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="58"/>
-      <c r="C10" s="60" t="s">
+    <row r="10" spans="2:24" ht="17.25" customHeight="1">
+      <c r="B10" s="57"/>
+      <c r="C10" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="61"/>
-      <c r="E10" s="62"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="40"/>
       <c r="F10" s="21" t="s">
         <v>48</v>
       </c>
@@ -1598,11 +1599,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="58"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="65"/>
+    <row r="11" spans="2:24" ht="17.25" customHeight="1">
+      <c r="B11" s="57"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="43"/>
       <c r="F11" s="28" t="s">
         <v>49</v>
       </c>
@@ -1621,13 +1622,13 @@
       <c r="S11" s="27"/>
       <c r="T11" s="28"/>
     </row>
-    <row r="12" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="58"/>
-      <c r="C12" s="60" t="s">
+    <row r="12" spans="2:24" ht="17.25" customHeight="1">
+      <c r="B12" s="57"/>
+      <c r="C12" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="61"/>
-      <c r="E12" s="62"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="40"/>
       <c r="F12" s="21" t="s">
         <v>50</v>
       </c>
@@ -1646,11 +1647,11 @@
       <c r="S12" s="20"/>
       <c r="T12" s="21"/>
     </row>
-    <row r="13" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="58"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="65"/>
+    <row r="13" spans="2:24" ht="17.25" customHeight="1">
+      <c r="B13" s="57"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="43"/>
       <c r="F13" s="28" t="s">
         <v>51</v>
       </c>
@@ -1669,13 +1670,13 @@
       <c r="S13" s="27"/>
       <c r="T13" s="28"/>
     </row>
-    <row r="14" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="58"/>
-      <c r="C14" s="60" t="s">
+    <row r="14" spans="2:24" ht="17.25" customHeight="1">
+      <c r="B14" s="57"/>
+      <c r="C14" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="61"/>
-      <c r="E14" s="62"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="40"/>
       <c r="F14" s="21" t="s">
         <v>47</v>
       </c>
@@ -1694,11 +1695,11 @@
       <c r="S14" s="20"/>
       <c r="T14" s="21"/>
     </row>
-    <row r="15" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="59"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="65"/>
+    <row r="15" spans="2:24" ht="17.25" customHeight="1">
+      <c r="B15" s="58"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="43"/>
       <c r="F15" s="28" t="s">
         <v>52</v>
       </c>
@@ -1717,15 +1718,15 @@
       <c r="S15" s="27"/>
       <c r="T15" s="28"/>
     </row>
-    <row r="16" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="48" t="s">
+    <row r="16" spans="2:24" ht="17.25" customHeight="1">
+      <c r="B16" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="55" t="s">
+      <c r="C16" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
       <c r="F16" s="3" t="s">
         <v>15</v>
       </c>
@@ -1744,13 +1745,13 @@
       <c r="S16" s="2"/>
       <c r="T16" s="3"/>
     </row>
-    <row r="17" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="48"/>
-      <c r="C17" s="55" t="s">
+    <row r="17" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B17" s="46"/>
+      <c r="C17" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="55"/>
-      <c r="E17" s="55"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
       <c r="F17" s="3" t="s">
         <v>15</v>
       </c>
@@ -1769,8 +1770,8 @@
       <c r="S17" s="2"/>
       <c r="T17" s="3"/>
     </row>
-    <row r="18" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="49" t="s">
+    <row r="18" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B18" s="70" t="s">
         <v>46</v>
       </c>
       <c r="C18" s="51" t="s">
@@ -1800,8 +1801,8 @@
       <c r="S18" s="22"/>
       <c r="T18" s="23"/>
     </row>
-    <row r="19" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="49"/>
+    <row r="19" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B19" s="70"/>
       <c r="C19" s="52"/>
       <c r="D19" s="52"/>
       <c r="E19" s="7" t="s">
@@ -1825,8 +1826,8 @@
       <c r="S19" s="22"/>
       <c r="T19" s="23"/>
     </row>
-    <row r="20" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="49"/>
+    <row r="20" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B20" s="70"/>
       <c r="C20" s="52"/>
       <c r="D20" s="52"/>
       <c r="E20" s="7" t="s">
@@ -1850,8 +1851,8 @@
       <c r="S20" s="22"/>
       <c r="T20" s="23"/>
     </row>
-    <row r="21" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="49"/>
+    <row r="21" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B21" s="70"/>
       <c r="C21" s="52"/>
       <c r="D21" s="52"/>
       <c r="E21" s="7" t="s">
@@ -1875,8 +1876,8 @@
       <c r="S21" s="22"/>
       <c r="T21" s="23"/>
     </row>
-    <row r="22" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="49"/>
+    <row r="22" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B22" s="70"/>
       <c r="C22" s="52"/>
       <c r="D22" s="53"/>
       <c r="E22" s="7" t="s">
@@ -1894,14 +1895,14 @@
       <c r="M22" s="31"/>
       <c r="N22" s="11"/>
       <c r="O22" s="31"/>
-      <c r="P22" s="15"/>
+      <c r="P22" s="37"/>
       <c r="Q22" s="15"/>
-      <c r="R22" s="31"/>
+      <c r="R22" s="15"/>
       <c r="S22" s="31"/>
       <c r="T22" s="32"/>
     </row>
-    <row r="23" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="49"/>
+    <row r="23" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B23" s="70"/>
       <c r="C23" s="52"/>
       <c r="D23" s="51" t="s">
         <v>57</v>
@@ -1923,12 +1924,12 @@
       <c r="O23" s="22"/>
       <c r="P23" s="22"/>
       <c r="Q23" s="22"/>
-      <c r="R23" s="22"/>
+      <c r="R23" s="37"/>
       <c r="S23" s="22"/>
       <c r="T23" s="23"/>
     </row>
-    <row r="24" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="49"/>
+    <row r="24" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B24" s="70"/>
       <c r="C24" s="52"/>
       <c r="D24" s="52"/>
       <c r="E24" s="7" t="s">
@@ -1948,12 +1949,12 @@
       <c r="O24" s="22"/>
       <c r="P24" s="22"/>
       <c r="Q24" s="22"/>
-      <c r="R24" s="22"/>
+      <c r="R24" s="37"/>
       <c r="S24" s="22"/>
       <c r="T24" s="23"/>
     </row>
-    <row r="25" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="49"/>
+    <row r="25" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B25" s="70"/>
       <c r="C25" s="52"/>
       <c r="D25" s="52"/>
       <c r="E25" s="7" t="s">
@@ -1973,12 +1974,12 @@
       <c r="O25" s="33"/>
       <c r="P25" s="33"/>
       <c r="Q25" s="33"/>
-      <c r="R25" s="33"/>
+      <c r="R25" s="37"/>
       <c r="S25" s="33"/>
       <c r="T25" s="34"/>
     </row>
-    <row r="26" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="49"/>
+    <row r="26" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B26" s="70"/>
       <c r="C26" s="52"/>
       <c r="D26" s="52"/>
       <c r="E26" s="7" t="s">
@@ -1993,17 +1994,17 @@
       <c r="J26" s="2"/>
       <c r="K26" s="11"/>
       <c r="L26" s="11"/>
-      <c r="M26" s="19"/>
+      <c r="M26" s="11"/>
       <c r="N26" s="19"/>
-      <c r="O26" s="2"/>
+      <c r="O26" s="19"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
-      <c r="R26" s="2"/>
+      <c r="R26" s="37"/>
       <c r="S26" s="2"/>
       <c r="T26" s="3"/>
     </row>
-    <row r="27" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="49"/>
+    <row r="27" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B27" s="70"/>
       <c r="C27" s="52"/>
       <c r="D27" s="53"/>
       <c r="E27" s="7" t="s">
@@ -2021,19 +2022,19 @@
       <c r="M27" s="11"/>
       <c r="N27" s="11"/>
       <c r="O27" s="31"/>
-      <c r="P27" s="15"/>
+      <c r="P27" s="37"/>
       <c r="Q27" s="15"/>
-      <c r="R27" s="31"/>
+      <c r="R27" s="15"/>
       <c r="S27" s="31"/>
       <c r="T27" s="32"/>
     </row>
-    <row r="28" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="49"/>
+    <row r="28" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B28" s="70"/>
       <c r="C28" s="53"/>
-      <c r="D28" s="55" t="s">
+      <c r="D28" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="E28" s="55"/>
+      <c r="E28" s="54"/>
       <c r="F28" s="3" t="s">
         <v>38</v>
       </c>
@@ -2046,18 +2047,18 @@
       <c r="M28" s="17"/>
       <c r="N28" s="17"/>
       <c r="O28" s="17"/>
-      <c r="P28" s="14"/>
+      <c r="P28" s="37"/>
       <c r="Q28" s="14"/>
-      <c r="R28" s="2"/>
+      <c r="R28" s="14"/>
       <c r="S28" s="2"/>
       <c r="T28" s="3"/>
     </row>
-    <row r="29" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="49"/>
+    <row r="29" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B29" s="70"/>
       <c r="C29" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="56" t="s">
+      <c r="D29" s="55" t="s">
         <v>61</v>
       </c>
       <c r="E29" s="7" t="s">
@@ -2081,10 +2082,10 @@
       <c r="S29" s="12"/>
       <c r="T29" s="13"/>
     </row>
-    <row r="30" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="49"/>
+    <row r="30" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B30" s="70"/>
       <c r="C30" s="52"/>
-      <c r="D30" s="56"/>
+      <c r="D30" s="55"/>
       <c r="E30" s="7" t="s">
         <v>64</v>
       </c>
@@ -2106,13 +2107,13 @@
       <c r="S30" s="12"/>
       <c r="T30" s="13"/>
     </row>
-    <row r="31" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="49"/>
+    <row r="31" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B31" s="70"/>
       <c r="C31" s="53"/>
-      <c r="D31" s="46" t="s">
+      <c r="D31" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="E31" s="47"/>
+      <c r="E31" s="69"/>
       <c r="F31" s="13" t="s">
         <v>38</v>
       </c>
@@ -2131,15 +2132,15 @@
       <c r="S31" s="12"/>
       <c r="T31" s="13"/>
     </row>
-    <row r="32" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="49"/>
+    <row r="32" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B32" s="70"/>
       <c r="C32" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="46" t="s">
+      <c r="D32" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="E32" s="47"/>
+      <c r="E32" s="69"/>
       <c r="F32" s="23" t="s">
         <v>40</v>
       </c>
@@ -2152,18 +2153,19 @@
       <c r="M32" s="11"/>
       <c r="N32" s="15"/>
       <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
       <c r="Q32" s="17"/>
       <c r="R32" s="17"/>
       <c r="S32" s="22"/>
       <c r="T32" s="23"/>
     </row>
-    <row r="33" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="49"/>
+    <row r="33" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B33" s="70"/>
       <c r="C33" s="52"/>
-      <c r="D33" s="46" t="s">
+      <c r="D33" s="68" t="s">
         <v>53</v>
       </c>
-      <c r="E33" s="47"/>
+      <c r="E33" s="69"/>
       <c r="F33" s="23" t="s">
         <v>38</v>
       </c>
@@ -2173,22 +2175,22 @@
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="36"/>
-      <c r="M33" s="36"/>
+      <c r="M33" s="11"/>
       <c r="N33" s="14"/>
       <c r="O33" s="14"/>
-      <c r="P33" s="12"/>
+      <c r="P33" s="14"/>
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
       <c r="S33" s="2"/>
       <c r="T33" s="3"/>
     </row>
-    <row r="34" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="49"/>
+    <row r="34" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B34" s="70"/>
       <c r="C34" s="52"/>
-      <c r="D34" s="46" t="s">
+      <c r="D34" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="E34" s="47"/>
+      <c r="E34" s="69"/>
       <c r="F34" s="23" t="s">
         <v>71</v>
       </c>
@@ -2201,19 +2203,19 @@
       <c r="M34" s="14"/>
       <c r="N34" s="14"/>
       <c r="O34" s="14"/>
-      <c r="P34" s="22"/>
+      <c r="P34" s="14"/>
       <c r="Q34" s="22"/>
       <c r="R34" s="22"/>
       <c r="S34" s="22"/>
       <c r="T34" s="23"/>
     </row>
-    <row r="35" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="49"/>
+    <row r="35" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B35" s="70"/>
       <c r="C35" s="52"/>
-      <c r="D35" s="46" t="s">
+      <c r="D35" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="E35" s="47"/>
+      <c r="E35" s="69"/>
       <c r="F35" s="23" t="s">
         <v>38</v>
       </c>
@@ -2232,13 +2234,13 @@
       <c r="S35" s="22"/>
       <c r="T35" s="23"/>
     </row>
-    <row r="36" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="49"/>
+    <row r="36" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B36" s="70"/>
       <c r="C36" s="53"/>
-      <c r="D36" s="46" t="s">
+      <c r="D36" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="E36" s="47"/>
+      <c r="E36" s="69"/>
       <c r="F36" s="23" t="s">
         <v>24</v>
       </c>
@@ -2257,13 +2259,13 @@
       <c r="S36" s="22"/>
       <c r="T36" s="23"/>
     </row>
-    <row r="37" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="49"/>
-      <c r="C37" s="40" t="s">
+    <row r="37" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B37" s="70"/>
+      <c r="C37" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="D37" s="41"/>
-      <c r="E37" s="42"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="64"/>
       <c r="F37" s="23" t="s">
         <v>23</v>
       </c>
@@ -2282,11 +2284,11 @@
       <c r="S37" s="22"/>
       <c r="T37" s="23"/>
     </row>
-    <row r="38" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="50"/>
-      <c r="C38" s="43"/>
-      <c r="D38" s="44"/>
-      <c r="E38" s="45"/>
+    <row r="38" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B38" s="71"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="66"/>
+      <c r="E38" s="67"/>
       <c r="F38" s="23" t="s">
         <v>40</v>
       </c>
@@ -2305,15 +2307,15 @@
       <c r="S38" s="22"/>
       <c r="T38" s="23"/>
     </row>
-    <row r="39" spans="2:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="48" t="s">
+    <row r="39" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B39" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="C39" s="46" t="s">
+      <c r="C39" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="D39" s="54"/>
-      <c r="E39" s="47"/>
+      <c r="D39" s="72"/>
+      <c r="E39" s="69"/>
       <c r="F39" s="23" t="s">
         <v>10</v>
       </c>
@@ -2328,17 +2330,17 @@
       <c r="O39" s="5"/>
       <c r="P39" s="5"/>
       <c r="Q39" s="5"/>
-      <c r="R39" s="22"/>
+      <c r="R39" s="5"/>
       <c r="S39" s="22"/>
       <c r="T39" s="23"/>
     </row>
-    <row r="40" spans="2:20" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B40" s="48"/>
-      <c r="C40" s="46" t="s">
+    <row r="40" spans="2:20" ht="17.25">
+      <c r="B40" s="46"/>
+      <c r="C40" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="D40" s="54"/>
-      <c r="E40" s="47"/>
+      <c r="D40" s="72"/>
+      <c r="E40" s="69"/>
       <c r="F40" s="23" t="s">
         <v>10</v>
       </c>
@@ -2357,13 +2359,13 @@
       <c r="S40" s="22"/>
       <c r="T40" s="23"/>
     </row>
-    <row r="41" spans="2:20" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B41" s="48"/>
-      <c r="C41" s="46" t="s">
+    <row r="41" spans="2:20" ht="17.25">
+      <c r="B41" s="46"/>
+      <c r="C41" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="54"/>
-      <c r="E41" s="47"/>
+      <c r="D41" s="72"/>
+      <c r="E41" s="69"/>
       <c r="F41" s="23" t="s">
         <v>10</v>
       </c>
@@ -2382,13 +2384,13 @@
       <c r="S41" s="5"/>
       <c r="T41" s="23"/>
     </row>
-    <row r="42" spans="2:20" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="37" t="s">
+    <row r="42" spans="2:20" ht="18" thickBot="1">
+      <c r="B42" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="39"/>
+      <c r="C42" s="60"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="61"/>
       <c r="F42" s="8" t="s">
         <v>15</v>
       </c>
@@ -2407,7 +2409,7 @@
       <c r="S42" s="9"/>
       <c r="T42" s="10"/>
     </row>
-    <row r="43" spans="2:20" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:20" ht="17.25">
       <c r="E43" s="29"/>
       <c r="F43" s="29"/>
       <c r="G43" s="29"/>
@@ -2425,7 +2427,7 @@
       <c r="S43" s="29"/>
       <c r="T43" s="29"/>
     </row>
-    <row r="45" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:20">
       <c r="L45" t="s">
         <v>33</v>
       </c>
@@ -2441,14 +2443,22 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="C14:E15"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="B2:E3"/>
-    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="C37:E38"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B18:B38"/>
+    <mergeCell ref="C18:C28"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C32:C36"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
     <mergeCell ref="D23:D27"/>
     <mergeCell ref="D18:D22"/>
     <mergeCell ref="D28:E28"/>
@@ -2465,22 +2475,14 @@
     <mergeCell ref="B7:B15"/>
     <mergeCell ref="C10:E11"/>
     <mergeCell ref="C12:E13"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="C37:E38"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B18:B38"/>
-    <mergeCell ref="C18:C28"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="C32:C36"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="C14:E15"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B2:E3"/>
+    <mergeCell ref="G2:J2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2489,12 +2491,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2502,12 +2504,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new file:   Documents/presentation doc/mid_presentation.pptx
</commit_message>
<xml_diff>
--- a/Documents/proposal/Project plan.xlsx
+++ b/Documents/proposal/Project plan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
   <si>
     <t>주제 선정</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -155,31 +155,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ProtoType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>중간1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>중간2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>최종</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>인구</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>윤재</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -883,6 +863,78 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -913,83 +965,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1300,10 +1280,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:X46"/>
+  <dimension ref="B1:T44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S32" sqref="S32"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:XFD46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1315,49 +1295,47 @@
     <col min="5" max="5" width="13.75" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="20" width="4" customWidth="1"/>
-    <col min="21" max="21" width="3.125" customWidth="1"/>
-    <col min="23" max="23" width="5.75" customWidth="1"/>
-    <col min="24" max="24" width="2.5" customWidth="1"/>
+    <col min="21" max="21" width="3.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24" ht="12" customHeight="1" thickBot="1"/>
-    <row r="2" spans="2:24" ht="17.25" customHeight="1">
-      <c r="B2" s="71"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="68" t="s">
+    <row r="1" spans="2:20" ht="12" customHeight="1" thickBot="1"/>
+    <row r="2" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B2" s="58"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="72" t="s">
+      <c r="G2" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67" t="s">
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67" t="s">
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="67"/>
-      <c r="S2" s="67" t="s">
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="T2" s="68"/>
-    </row>
-    <row r="3" spans="2:24" ht="17.25" customHeight="1">
-      <c r="B3" s="51"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="70"/>
+      <c r="T2" s="54"/>
+    </row>
+    <row r="3" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B3" s="55"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="57"/>
       <c r="G3" s="1">
         <v>1</v>
       </c>
@@ -1401,13 +1379,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:24" ht="17.25" customHeight="1">
-      <c r="B4" s="51" t="s">
+    <row r="4" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B4" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
       <c r="F4" s="3" t="s">
         <v>15</v>
       </c>
@@ -1426,15 +1404,15 @@
       <c r="S4" s="2"/>
       <c r="T4" s="3"/>
     </row>
-    <row r="5" spans="2:24" ht="17.25" customHeight="1">
-      <c r="B5" s="51" t="s">
+    <row r="5" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B5" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
       <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1453,13 +1431,13 @@
       <c r="S5" s="2"/>
       <c r="T5" s="3"/>
     </row>
-    <row r="6" spans="2:24" ht="17.25" customHeight="1">
-      <c r="B6" s="51"/>
-      <c r="C6" s="56" t="s">
+    <row r="6" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B6" s="55"/>
+      <c r="C6" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
       <c r="F6" s="3" t="s">
         <v>15</v>
       </c>
@@ -1478,15 +1456,15 @@
       <c r="S6" s="2"/>
       <c r="T6" s="3"/>
     </row>
-    <row r="7" spans="2:24" ht="17.25" customHeight="1">
-      <c r="B7" s="58" t="s">
+    <row r="7" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B7" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="56" t="s">
+      <c r="C7" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
       <c r="F7" s="3" t="s">
         <v>10</v>
       </c>
@@ -1504,22 +1482,14 @@
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
       <c r="T7" s="3"/>
-      <c r="V7" s="18"/>
-      <c r="W7" t="s">
-        <v>39</v>
-      </c>
-      <c r="X7">
-        <f>COUNTIF($F$18:$F$40,W7)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="2:24" ht="17.25" customHeight="1">
-      <c r="B8" s="59"/>
-      <c r="C8" s="56" t="s">
+    </row>
+    <row r="8" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B8" s="62"/>
+      <c r="C8" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
       <c r="F8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1537,22 +1507,14 @@
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
       <c r="T8" s="3"/>
-      <c r="V8" s="19"/>
-      <c r="W8" t="s">
-        <v>37</v>
-      </c>
-      <c r="X8">
-        <f>COUNTIF($F$18:$F$40,W8)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="2:24" ht="17.25" customHeight="1">
-      <c r="B9" s="59"/>
-      <c r="C9" s="56" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
+    </row>
+    <row r="9" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B9" s="62"/>
+      <c r="C9" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
       <c r="F9" s="3" t="s">
         <v>10</v>
       </c>
@@ -1570,24 +1532,16 @@
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
       <c r="T9" s="3"/>
-      <c r="V9" s="15"/>
-      <c r="W9" t="s">
-        <v>40</v>
-      </c>
-      <c r="X9">
-        <f>COUNTIF($F$18:$F$40,W9)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="2:24" ht="17.25" customHeight="1">
-      <c r="B10" s="59"/>
-      <c r="C10" s="61" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="62"/>
-      <c r="E10" s="63"/>
+    </row>
+    <row r="10" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B10" s="62"/>
+      <c r="C10" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="48"/>
+      <c r="E10" s="49"/>
       <c r="F10" s="21" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G10" s="25"/>
       <c r="H10" s="6"/>
@@ -1603,22 +1557,14 @@
       <c r="R10" s="20"/>
       <c r="S10" s="20"/>
       <c r="T10" s="21"/>
-      <c r="V10" s="14"/>
-      <c r="W10" t="s">
-        <v>38</v>
-      </c>
-      <c r="X10">
-        <f>COUNTIF($F$18:$F$40,W10)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="2:24" ht="17.25" customHeight="1">
-      <c r="B11" s="59"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="66"/>
+    </row>
+    <row r="11" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B11" s="62"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="52"/>
       <c r="F11" s="28" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G11" s="25"/>
       <c r="H11" s="6"/>
@@ -1635,15 +1581,15 @@
       <c r="S11" s="27"/>
       <c r="T11" s="28"/>
     </row>
-    <row r="12" spans="2:24" ht="17.25" customHeight="1">
-      <c r="B12" s="59"/>
-      <c r="C12" s="61" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="62"/>
-      <c r="E12" s="63"/>
+    <row r="12" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B12" s="62"/>
+      <c r="C12" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="48"/>
+      <c r="E12" s="49"/>
       <c r="F12" s="21" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G12" s="25"/>
       <c r="H12" s="6"/>
@@ -1660,13 +1606,13 @@
       <c r="S12" s="20"/>
       <c r="T12" s="21"/>
     </row>
-    <row r="13" spans="2:24" ht="17.25" customHeight="1">
-      <c r="B13" s="59"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="66"/>
+    <row r="13" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B13" s="62"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="52"/>
       <c r="F13" s="28" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G13" s="25"/>
       <c r="H13" s="6"/>
@@ -1683,15 +1629,15 @@
       <c r="S13" s="27"/>
       <c r="T13" s="28"/>
     </row>
-    <row r="14" spans="2:24" ht="17.25" customHeight="1">
-      <c r="B14" s="59"/>
-      <c r="C14" s="61" t="s">
+    <row r="14" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B14" s="62"/>
+      <c r="C14" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="48"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="21" t="s">
         <v>42</v>
-      </c>
-      <c r="D14" s="62"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="21" t="s">
-        <v>47</v>
       </c>
       <c r="G14" s="25"/>
       <c r="H14" s="6"/>
@@ -1708,13 +1654,13 @@
       <c r="S14" s="20"/>
       <c r="T14" s="21"/>
     </row>
-    <row r="15" spans="2:24" ht="17.25" customHeight="1">
-      <c r="B15" s="60"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="66"/>
+    <row r="15" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B15" s="63"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="52"/>
       <c r="F15" s="28" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G15" s="25"/>
       <c r="H15" s="6"/>
@@ -1731,15 +1677,15 @@
       <c r="S15" s="27"/>
       <c r="T15" s="28"/>
     </row>
-    <row r="16" spans="2:24" ht="17.25" customHeight="1">
-      <c r="B16" s="51" t="s">
+    <row r="16" spans="2:20" ht="17.25" customHeight="1">
+      <c r="B16" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="56" t="s">
+      <c r="C16" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
       <c r="F16" s="3" t="s">
         <v>15</v>
       </c>
@@ -1759,12 +1705,12 @@
       <c r="T16" s="3"/>
     </row>
     <row r="17" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B17" s="51"/>
-      <c r="C17" s="56" t="s">
+      <c r="B17" s="55"/>
+      <c r="C17" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
       <c r="F17" s="3" t="s">
         <v>15</v>
       </c>
@@ -1784,17 +1730,17 @@
       <c r="T17" s="3"/>
     </row>
     <row r="18" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B18" s="73" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="52" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="52" t="s">
-        <v>62</v>
+      <c r="B18" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="43" t="s">
+        <v>57</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F18" s="23" t="s">
         <v>23</v>
@@ -1815,11 +1761,11 @@
       <c r="T18" s="23"/>
     </row>
     <row r="19" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B19" s="74"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
       <c r="E19" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F19" s="23" t="s">
         <v>23</v>
@@ -1840,11 +1786,11 @@
       <c r="T19" s="23"/>
     </row>
     <row r="20" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B20" s="74"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
       <c r="E20" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F20" s="23" t="s">
         <v>23</v>
@@ -1865,11 +1811,11 @@
       <c r="T20" s="23"/>
     </row>
     <row r="21" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B21" s="74"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
       <c r="E21" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F21" s="23" t="s">
         <v>23</v>
@@ -1890,14 +1836,14 @@
       <c r="T21" s="23"/>
     </row>
     <row r="22" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B22" s="74"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="54"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="45"/>
       <c r="E22" s="7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F22" s="32" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G22" s="24"/>
       <c r="H22" s="31"/>
@@ -1915,13 +1861,13 @@
       <c r="T22" s="32"/>
     </row>
     <row r="23" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B23" s="74"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="52" t="s">
-        <v>57</v>
+      <c r="B23" s="41"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="43" t="s">
+        <v>52</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F23" s="23" t="s">
         <v>24</v>
@@ -1942,11 +1888,11 @@
       <c r="T23" s="23"/>
     </row>
     <row r="24" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B24" s="74"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
       <c r="E24" s="7" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F24" s="23" t="s">
         <v>24</v>
@@ -1967,14 +1913,14 @@
       <c r="T24" s="23"/>
     </row>
     <row r="25" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B25" s="74"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
       <c r="E25" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F25" s="34" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G25" s="24"/>
       <c r="H25" s="33"/>
@@ -1992,11 +1938,11 @@
       <c r="T25" s="34"/>
     </row>
     <row r="26" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B26" s="74"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
       <c r="E26" s="7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F26" s="23" t="s">
         <v>24</v>
@@ -2017,14 +1963,14 @@
       <c r="T26" s="3"/>
     </row>
     <row r="27" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B27" s="74"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="54"/>
+      <c r="B27" s="41"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="45"/>
       <c r="E27" s="7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F27" s="32" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G27" s="24"/>
       <c r="H27" s="31"/>
@@ -2042,14 +1988,14 @@
       <c r="T27" s="32"/>
     </row>
     <row r="28" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B28" s="74"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="56" t="s">
+      <c r="B28" s="41"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="E28" s="56"/>
+      <c r="E28" s="46"/>
       <c r="F28" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="2"/>
@@ -2067,18 +2013,18 @@
       <c r="T28" s="3"/>
     </row>
     <row r="29" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B29" s="74"/>
-      <c r="C29" s="52" t="s">
+      <c r="B29" s="41"/>
+      <c r="C29" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="57" t="s">
-        <v>61</v>
+      <c r="D29" s="60" t="s">
+        <v>56</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="12"/>
@@ -2096,11 +2042,11 @@
       <c r="T29" s="13"/>
     </row>
     <row r="30" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B30" s="74"/>
-      <c r="C30" s="53"/>
-      <c r="D30" s="57"/>
+      <c r="B30" s="41"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="60"/>
       <c r="E30" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F30" s="13" t="s">
         <v>23</v>
@@ -2121,14 +2067,14 @@
       <c r="T30" s="13"/>
     </row>
     <row r="31" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B31" s="74"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="49" t="s">
+      <c r="B31" s="41"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="E31" s="50"/>
+      <c r="E31" s="75"/>
       <c r="F31" s="13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="12"/>
@@ -2146,16 +2092,16 @@
       <c r="T31" s="13"/>
     </row>
     <row r="32" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B32" s="74"/>
-      <c r="C32" s="52" t="s">
+      <c r="B32" s="41"/>
+      <c r="C32" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="56" t="s">
-        <v>72</v>
-      </c>
-      <c r="E32" s="56"/>
+      <c r="D32" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" s="46"/>
       <c r="F32" s="39" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G32" s="24"/>
       <c r="H32" s="38"/>
@@ -2173,14 +2119,14 @@
       <c r="T32" s="39"/>
     </row>
     <row r="33" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B33" s="74"/>
-      <c r="C33" s="53"/>
-      <c r="D33" s="56" t="s">
+      <c r="B33" s="41"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="E33" s="56"/>
+      <c r="E33" s="46"/>
       <c r="F33" s="23" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G33" s="24"/>
       <c r="H33" s="22"/>
@@ -2198,14 +2144,14 @@
       <c r="T33" s="23"/>
     </row>
     <row r="34" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B34" s="74"/>
-      <c r="C34" s="53"/>
-      <c r="D34" s="56" t="s">
-        <v>53</v>
-      </c>
-      <c r="E34" s="56"/>
+      <c r="B34" s="41"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="46"/>
       <c r="F34" s="23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="2"/>
@@ -2223,14 +2169,14 @@
       <c r="T34" s="3"/>
     </row>
     <row r="35" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B35" s="74"/>
-      <c r="C35" s="53"/>
-      <c r="D35" s="56" t="s">
+      <c r="B35" s="41"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="E35" s="56"/>
+      <c r="E35" s="46"/>
       <c r="F35" s="23" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G35" s="24"/>
       <c r="H35" s="22"/>
@@ -2248,14 +2194,14 @@
       <c r="T35" s="23"/>
     </row>
     <row r="36" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B36" s="74"/>
-      <c r="C36" s="53"/>
-      <c r="D36" s="56" t="s">
+      <c r="B36" s="41"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="56"/>
+      <c r="E36" s="46"/>
       <c r="F36" s="23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G36" s="24"/>
       <c r="H36" s="22"/>
@@ -2273,12 +2219,12 @@
       <c r="T36" s="23"/>
     </row>
     <row r="37" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B37" s="74"/>
-      <c r="C37" s="54"/>
-      <c r="D37" s="56" t="s">
+      <c r="B37" s="41"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="E37" s="56"/>
+      <c r="E37" s="46"/>
       <c r="F37" s="23" t="s">
         <v>24</v>
       </c>
@@ -2298,12 +2244,12 @@
       <c r="T37" s="23"/>
     </row>
     <row r="38" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B38" s="74"/>
-      <c r="C38" s="43" t="s">
+      <c r="B38" s="41"/>
+      <c r="C38" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="D38" s="44"/>
-      <c r="E38" s="45"/>
+      <c r="D38" s="68"/>
+      <c r="E38" s="69"/>
       <c r="F38" s="23" t="s">
         <v>23</v>
       </c>
@@ -2323,12 +2269,12 @@
       <c r="T38" s="23"/>
     </row>
     <row r="39" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B39" s="75"/>
-      <c r="C39" s="46"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="48"/>
+      <c r="B39" s="42"/>
+      <c r="C39" s="70"/>
+      <c r="D39" s="71"/>
+      <c r="E39" s="72"/>
       <c r="F39" s="23" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G39" s="24"/>
       <c r="H39" s="22"/>
@@ -2346,14 +2292,14 @@
       <c r="T39" s="23"/>
     </row>
     <row r="40" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B40" s="51" t="s">
+      <c r="B40" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="49" t="s">
+      <c r="C40" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="D40" s="55"/>
-      <c r="E40" s="50"/>
+      <c r="D40" s="74"/>
+      <c r="E40" s="75"/>
       <c r="F40" s="23" t="s">
         <v>10</v>
       </c>
@@ -2373,12 +2319,12 @@
       <c r="T40" s="23"/>
     </row>
     <row r="41" spans="2:20" ht="17.25">
-      <c r="B41" s="51"/>
-      <c r="C41" s="49" t="s">
+      <c r="B41" s="55"/>
+      <c r="C41" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="D41" s="55"/>
-      <c r="E41" s="50"/>
+      <c r="D41" s="74"/>
+      <c r="E41" s="75"/>
       <c r="F41" s="23" t="s">
         <v>10</v>
       </c>
@@ -2398,12 +2344,12 @@
       <c r="T41" s="23"/>
     </row>
     <row r="42" spans="2:20" ht="17.25">
-      <c r="B42" s="51"/>
-      <c r="C42" s="49" t="s">
+      <c r="B42" s="55"/>
+      <c r="C42" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="D42" s="55"/>
-      <c r="E42" s="50"/>
+      <c r="D42" s="74"/>
+      <c r="E42" s="75"/>
       <c r="F42" s="23" t="s">
         <v>10</v>
       </c>
@@ -2423,12 +2369,12 @@
       <c r="T42" s="23"/>
     </row>
     <row r="43" spans="2:20" ht="18" thickBot="1">
-      <c r="B43" s="40" t="s">
+      <c r="B43" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="C43" s="41"/>
-      <c r="D43" s="41"/>
-      <c r="E43" s="42"/>
+      <c r="C43" s="65"/>
+      <c r="D43" s="65"/>
+      <c r="E43" s="66"/>
       <c r="F43" s="8" t="s">
         <v>15</v>
       </c>
@@ -2465,36 +2411,17 @@
       <c r="S44" s="29"/>
       <c r="T44" s="29"/>
     </row>
-    <row r="46" spans="2:20">
-      <c r="L46" t="s">
-        <v>33</v>
-      </c>
-      <c r="P46" t="s">
-        <v>34</v>
-      </c>
-      <c r="R46" t="s">
-        <v>35</v>
-      </c>
-      <c r="T46" t="s">
-        <v>36</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="C32:C37"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="C14:E15"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="B2:E3"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="D23:D27"/>
-    <mergeCell ref="D18:D22"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="C38:E39"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C6:E6"/>
@@ -2507,17 +2434,22 @@
     <mergeCell ref="B7:B15"/>
     <mergeCell ref="C10:E11"/>
     <mergeCell ref="C12:E13"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="C38:E39"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B2:E3"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="C32:C37"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="C14:E15"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="D23:D27"/>
+    <mergeCell ref="D18:D22"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:D30"/>
     <mergeCell ref="C18:C28"/>
     <mergeCell ref="C29:C31"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
     <mergeCell ref="D31:E31"/>
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="D34:E34"/>

</xml_diff>

<commit_message>
new file:   Documents/weekly report/JongUk Kim/Weekly report_JongUk-Kim_20120524.docx
</commit_message>
<xml_diff>
--- a/Documents/proposal/Project plan.xlsx
+++ b/Documents/proposal/Project plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="30" windowWidth="20730" windowHeight="10020"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="70">
   <si>
     <t>주제 선정</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -127,19 +127,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Device Driver</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Device Driver</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>USB/IP Porting</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VHCI Driver</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -296,6 +284,26 @@
   </si>
   <si>
     <t>Odroid 터미널에서 실행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VHCI Driver</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stub_driver.c 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bind-driver.c 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -742,7 +750,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -863,6 +871,81 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -875,101 +958,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1283,7 +1297,7 @@
   <dimension ref="B1:T44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E3"/>
+      <selection activeCell="B18" sqref="B18:B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1300,42 +1314,42 @@
   <sheetData>
     <row r="1" spans="2:20" ht="12" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B2" s="67"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="64" t="s">
+      <c r="B2" s="54"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="68" t="s">
+      <c r="G2" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63" t="s">
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63"/>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63" t="s">
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63" t="s">
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="T2" s="64"/>
+      <c r="T2" s="50"/>
     </row>
     <row r="3" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B3" s="50"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="66"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="53"/>
       <c r="G3" s="1">
         <v>1</v>
       </c>
@@ -1379,13 +1393,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B4" s="50" t="s">
+    <row r="4" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B4" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
       <c r="F4" s="3" t="s">
         <v>15</v>
       </c>
@@ -1404,15 +1418,15 @@
       <c r="S4" s="2"/>
       <c r="T4" s="3"/>
     </row>
-    <row r="5" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B5" s="50" t="s">
+    <row r="5" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B5" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
       <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1431,13 +1445,13 @@
       <c r="S5" s="2"/>
       <c r="T5" s="3"/>
     </row>
-    <row r="6" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B6" s="50"/>
-      <c r="C6" s="49" t="s">
+    <row r="6" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B6" s="51"/>
+      <c r="C6" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
       <c r="F6" s="3" t="s">
         <v>15</v>
       </c>
@@ -1456,15 +1470,15 @@
       <c r="S6" s="2"/>
       <c r="T6" s="3"/>
     </row>
-    <row r="7" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B7" s="54" t="s">
+    <row r="7" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B7" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
       <c r="F7" s="3" t="s">
         <v>10</v>
       </c>
@@ -1483,13 +1497,13 @@
       <c r="S7" s="2"/>
       <c r="T7" s="3"/>
     </row>
-    <row r="8" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B8" s="55"/>
-      <c r="C8" s="49" t="s">
+    <row r="8" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B8" s="57"/>
+      <c r="C8" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
       <c r="F8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1508,13 +1522,13 @@
       <c r="S8" s="2"/>
       <c r="T8" s="3"/>
     </row>
-    <row r="9" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B9" s="55"/>
-      <c r="C9" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
+    <row r="9" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B9" s="57"/>
+      <c r="C9" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
       <c r="F9" s="3" t="s">
         <v>10</v>
       </c>
@@ -1533,15 +1547,15 @@
       <c r="S9" s="2"/>
       <c r="T9" s="3"/>
     </row>
-    <row r="10" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B10" s="55"/>
-      <c r="C10" s="57" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="58"/>
-      <c r="E10" s="59"/>
+    <row r="10" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B10" s="57"/>
+      <c r="C10" s="59" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="60"/>
+      <c r="E10" s="61"/>
       <c r="F10" s="21" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G10" s="25"/>
       <c r="H10" s="6"/>
@@ -1558,13 +1572,13 @@
       <c r="S10" s="20"/>
       <c r="T10" s="21"/>
     </row>
-    <row r="11" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B11" s="55"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="62"/>
+    <row r="11" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B11" s="57"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="64"/>
       <c r="F11" s="28" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G11" s="25"/>
       <c r="H11" s="6"/>
@@ -1581,15 +1595,15 @@
       <c r="S11" s="27"/>
       <c r="T11" s="28"/>
     </row>
-    <row r="12" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B12" s="55"/>
-      <c r="C12" s="57" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="58"/>
-      <c r="E12" s="59"/>
+    <row r="12" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B12" s="57"/>
+      <c r="C12" s="59" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="60"/>
+      <c r="E12" s="61"/>
       <c r="F12" s="21" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G12" s="25"/>
       <c r="H12" s="6"/>
@@ -1606,13 +1620,13 @@
       <c r="S12" s="20"/>
       <c r="T12" s="21"/>
     </row>
-    <row r="13" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B13" s="55"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="62"/>
+    <row r="13" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B13" s="57"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="64"/>
       <c r="F13" s="28" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G13" s="25"/>
       <c r="H13" s="6"/>
@@ -1629,15 +1643,15 @@
       <c r="S13" s="27"/>
       <c r="T13" s="28"/>
     </row>
-    <row r="14" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B14" s="55"/>
-      <c r="C14" s="57" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="58"/>
-      <c r="E14" s="59"/>
+    <row r="14" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B14" s="57"/>
+      <c r="C14" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="60"/>
+      <c r="E14" s="61"/>
       <c r="F14" s="21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G14" s="25"/>
       <c r="H14" s="6"/>
@@ -1654,13 +1668,13 @@
       <c r="S14" s="20"/>
       <c r="T14" s="21"/>
     </row>
-    <row r="15" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B15" s="56"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="62"/>
+    <row r="15" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B15" s="58"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="64"/>
       <c r="F15" s="28" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G15" s="25"/>
       <c r="H15" s="6"/>
@@ -1677,15 +1691,15 @@
       <c r="S15" s="27"/>
       <c r="T15" s="28"/>
     </row>
-    <row r="16" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B16" s="50" t="s">
+    <row r="16" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B16" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="49" t="s">
+      <c r="C16" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
       <c r="F16" s="3" t="s">
         <v>15</v>
       </c>
@@ -1704,13 +1718,13 @@
       <c r="S16" s="2"/>
       <c r="T16" s="3"/>
     </row>
-    <row r="17" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B17" s="50"/>
-      <c r="C17" s="49" t="s">
+    <row r="17" spans="2:20" ht="17.25" hidden="1" customHeight="1">
+      <c r="B17" s="51"/>
+      <c r="C17" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
       <c r="F17" s="3" t="s">
         <v>15</v>
       </c>
@@ -1730,17 +1744,17 @@
       <c r="T17" s="3"/>
     </row>
     <row r="18" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B18" s="73" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="69" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="69" t="s">
-        <v>57</v>
+      <c r="B18" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="42" t="s">
+        <v>54</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F18" s="23" t="s">
         <v>23</v>
@@ -1761,11 +1775,11 @@
       <c r="T18" s="23"/>
     </row>
     <row r="19" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B19" s="74"/>
-      <c r="C19" s="70"/>
-      <c r="D19" s="70"/>
+      <c r="B19" s="71"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
       <c r="E19" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F19" s="23" t="s">
         <v>23</v>
@@ -1786,11 +1800,11 @@
       <c r="T19" s="23"/>
     </row>
     <row r="20" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B20" s="74"/>
-      <c r="C20" s="70"/>
-      <c r="D20" s="70"/>
+      <c r="B20" s="71"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
       <c r="E20" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F20" s="23" t="s">
         <v>23</v>
@@ -1811,11 +1825,11 @@
       <c r="T20" s="23"/>
     </row>
     <row r="21" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B21" s="74"/>
-      <c r="C21" s="70"/>
-      <c r="D21" s="70"/>
+      <c r="B21" s="71"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
       <c r="E21" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F21" s="23" t="s">
         <v>23</v>
@@ -1836,14 +1850,14 @@
       <c r="T21" s="23"/>
     </row>
     <row r="22" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B22" s="74"/>
-      <c r="C22" s="70"/>
-      <c r="D22" s="71"/>
+      <c r="B22" s="71"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="44"/>
       <c r="E22" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F22" s="32" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G22" s="24"/>
       <c r="H22" s="31"/>
@@ -1861,13 +1875,13 @@
       <c r="T22" s="32"/>
     </row>
     <row r="23" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B23" s="74"/>
-      <c r="C23" s="70"/>
-      <c r="D23" s="69" t="s">
-        <v>52</v>
+      <c r="B23" s="71"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="42" t="s">
+        <v>49</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F23" s="23" t="s">
         <v>24</v>
@@ -1888,11 +1902,11 @@
       <c r="T23" s="23"/>
     </row>
     <row r="24" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B24" s="74"/>
-      <c r="C24" s="70"/>
-      <c r="D24" s="70"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
       <c r="E24" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F24" s="23" t="s">
         <v>24</v>
@@ -1913,14 +1927,14 @@
       <c r="T24" s="23"/>
     </row>
     <row r="25" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B25" s="74"/>
-      <c r="C25" s="70"/>
-      <c r="D25" s="70"/>
+      <c r="B25" s="71"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
       <c r="E25" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F25" s="34" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G25" s="24"/>
       <c r="H25" s="33"/>
@@ -1938,11 +1952,11 @@
       <c r="T25" s="34"/>
     </row>
     <row r="26" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B26" s="74"/>
-      <c r="C26" s="70"/>
-      <c r="D26" s="70"/>
+      <c r="B26" s="71"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
       <c r="E26" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F26" s="23" t="s">
         <v>24</v>
@@ -1963,14 +1977,14 @@
       <c r="T26" s="3"/>
     </row>
     <row r="27" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B27" s="74"/>
-      <c r="C27" s="70"/>
-      <c r="D27" s="71"/>
+      <c r="B27" s="71"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="44"/>
       <c r="E27" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F27" s="32" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G27" s="24"/>
       <c r="H27" s="31"/>
@@ -1982,49 +1996,49 @@
       <c r="N27" s="11"/>
       <c r="O27" s="31"/>
       <c r="P27" s="37"/>
-      <c r="Q27" s="15"/>
+      <c r="Q27" s="40"/>
       <c r="R27" s="15"/>
       <c r="S27" s="31"/>
       <c r="T27" s="32"/>
     </row>
     <row r="28" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B28" s="74"/>
-      <c r="C28" s="71"/>
-      <c r="D28" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="49"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="F28" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G28" s="1"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="17"/>
-      <c r="O28" s="17"/>
-      <c r="P28" s="37"/>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="2"/>
-      <c r="T28" s="3"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="40"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="12"/>
+      <c r="T28" s="13"/>
     </row>
     <row r="29" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B29" s="74"/>
-      <c r="C29" s="69" t="s">
-        <v>25</v>
-      </c>
-      <c r="D29" s="72" t="s">
+      <c r="B29" s="71"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>33</v>
+      <c r="F29" s="13" t="s">
+        <v>23</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="12"/>
@@ -2035,221 +2049,221 @@
       <c r="M29" s="11"/>
       <c r="N29" s="11"/>
       <c r="O29" s="12"/>
-      <c r="P29" s="12"/>
-      <c r="Q29" s="19"/>
-      <c r="R29" s="19"/>
+      <c r="P29" s="40"/>
+      <c r="Q29" s="18"/>
+      <c r="R29" s="18"/>
       <c r="S29" s="12"/>
       <c r="T29" s="13"/>
     </row>
     <row r="30" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B30" s="74"/>
-      <c r="C30" s="70"/>
-      <c r="D30" s="72"/>
-      <c r="E30" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="G30" s="1"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
-      <c r="N30" s="11"/>
-      <c r="O30" s="12"/>
-      <c r="P30" s="12"/>
-      <c r="Q30" s="18"/>
-      <c r="R30" s="18"/>
-      <c r="S30" s="12"/>
-      <c r="T30" s="13"/>
+      <c r="B30" s="71"/>
+      <c r="C30" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" s="45"/>
+      <c r="F30" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" s="24"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
+      <c r="K30" s="38"/>
+      <c r="L30" s="38"/>
+      <c r="M30" s="38"/>
+      <c r="N30" s="38"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="38"/>
+      <c r="R30" s="38"/>
+      <c r="S30" s="38"/>
+      <c r="T30" s="39"/>
     </row>
     <row r="31" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B31" s="74"/>
-      <c r="C31" s="71"/>
-      <c r="D31" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="E31" s="53"/>
-      <c r="F31" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G31" s="1"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
+      <c r="B31" s="71"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="45"/>
+      <c r="F31" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G31" s="24"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
       <c r="K31" s="17"/>
       <c r="L31" s="17"/>
       <c r="M31" s="11"/>
-      <c r="N31" s="11"/>
-      <c r="O31" s="12"/>
-      <c r="P31" s="22"/>
-      <c r="Q31" s="14"/>
-      <c r="R31" s="14"/>
-      <c r="S31" s="12"/>
-      <c r="T31" s="13"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="17"/>
+      <c r="S31" s="22"/>
+      <c r="T31" s="23"/>
     </row>
     <row r="32" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B32" s="74"/>
-      <c r="C32" s="69" t="s">
-        <v>28</v>
-      </c>
-      <c r="D32" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="E32" s="49"/>
-      <c r="F32" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="G32" s="24"/>
-      <c r="H32" s="38"/>
-      <c r="I32" s="38"/>
-      <c r="J32" s="38"/>
-      <c r="K32" s="38"/>
-      <c r="L32" s="38"/>
-      <c r="M32" s="38"/>
-      <c r="N32" s="38"/>
-      <c r="O32" s="14"/>
+      <c r="B32" s="71"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" s="45"/>
+      <c r="F32" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G32" s="1"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="36"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
       <c r="P32" s="14"/>
-      <c r="Q32" s="38"/>
-      <c r="R32" s="38"/>
-      <c r="S32" s="38"/>
-      <c r="T32" s="39"/>
+      <c r="Q32" s="14"/>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="3"/>
     </row>
     <row r="33" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B33" s="74"/>
-      <c r="C33" s="70"/>
-      <c r="D33" s="49" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" s="49"/>
+      <c r="B33" s="71"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="45"/>
       <c r="F33" s="23" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="G33" s="24"/>
       <c r="H33" s="22"/>
       <c r="I33" s="22"/>
       <c r="J33" s="22"/>
-      <c r="K33" s="17"/>
-      <c r="L33" s="17"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="15"/>
-      <c r="O33" s="15"/>
-      <c r="P33" s="15"/>
-      <c r="Q33" s="17"/>
-      <c r="R33" s="17"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="27"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="14"/>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="22"/>
+      <c r="R33" s="22"/>
       <c r="S33" s="22"/>
       <c r="T33" s="23"/>
     </row>
     <row r="34" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B34" s="74"/>
-      <c r="C34" s="70"/>
-      <c r="D34" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="E34" s="49"/>
+      <c r="B34" s="71"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" s="45"/>
       <c r="F34" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="G34" s="1"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="36"/>
-      <c r="M34" s="11"/>
-      <c r="N34" s="11"/>
-      <c r="O34" s="11"/>
+        <v>31</v>
+      </c>
+      <c r="G34" s="24"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="14"/>
       <c r="P34" s="14"/>
-      <c r="Q34" s="14"/>
-      <c r="R34" s="2"/>
-      <c r="S34" s="2"/>
-      <c r="T34" s="3"/>
+      <c r="Q34" s="22"/>
+      <c r="R34" s="22"/>
+      <c r="S34" s="22"/>
+      <c r="T34" s="23"/>
     </row>
     <row r="35" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B35" s="74"/>
-      <c r="C35" s="70"/>
-      <c r="D35" s="49" t="s">
-        <v>30</v>
-      </c>
-      <c r="E35" s="49"/>
-      <c r="F35" s="23" t="s">
-        <v>66</v>
+      <c r="B35" s="71"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35" s="45"/>
+      <c r="F35" s="41" t="s">
+        <v>32</v>
       </c>
       <c r="G35" s="24"/>
       <c r="H35" s="22"/>
       <c r="I35" s="22"/>
       <c r="J35" s="22"/>
       <c r="K35" s="22"/>
-      <c r="L35" s="27"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14"/>
-      <c r="P35" s="14"/>
-      <c r="Q35" s="22"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="35"/>
+      <c r="N35" s="40"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="40"/>
       <c r="R35" s="22"/>
       <c r="S35" s="22"/>
       <c r="T35" s="23"/>
     </row>
     <row r="36" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B36" s="74"/>
-      <c r="C36" s="70"/>
-      <c r="D36" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="E36" s="49"/>
-      <c r="F36" s="23" t="s">
-        <v>34</v>
+      <c r="B36" s="71"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="E36" s="45"/>
+      <c r="F36" s="41" t="s">
+        <v>69</v>
       </c>
       <c r="G36" s="24"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="22"/>
-      <c r="J36" s="22"/>
-      <c r="K36" s="22"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="14"/>
-      <c r="O36" s="14"/>
-      <c r="P36" s="14"/>
-      <c r="Q36" s="22"/>
-      <c r="R36" s="22"/>
-      <c r="S36" s="22"/>
-      <c r="T36" s="23"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="40"/>
+      <c r="K36" s="40"/>
+      <c r="L36" s="40"/>
+      <c r="M36" s="40"/>
+      <c r="N36" s="40"/>
+      <c r="O36" s="40"/>
+      <c r="P36" s="18"/>
+      <c r="Q36" s="18"/>
+      <c r="R36" s="40"/>
+      <c r="S36" s="40"/>
+      <c r="T36" s="41"/>
     </row>
     <row r="37" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B37" s="74"/>
-      <c r="C37" s="71"/>
-      <c r="D37" s="49" t="s">
-        <v>32</v>
-      </c>
-      <c r="E37" s="49"/>
-      <c r="F37" s="23" t="s">
-        <v>24</v>
+      <c r="B37" s="71"/>
+      <c r="C37" s="44"/>
+      <c r="D37" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="E37" s="45"/>
+      <c r="F37" s="41" t="s">
+        <v>68</v>
       </c>
       <c r="G37" s="24"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
-      <c r="J37" s="22"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="22"/>
-      <c r="M37" s="35"/>
-      <c r="N37" s="19"/>
-      <c r="O37" s="19"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40"/>
+      <c r="K37" s="40"/>
+      <c r="L37" s="40"/>
+      <c r="M37" s="40"/>
+      <c r="N37" s="40"/>
+      <c r="O37" s="40"/>
       <c r="P37" s="19"/>
-      <c r="Q37" s="22"/>
-      <c r="R37" s="22"/>
-      <c r="S37" s="22"/>
-      <c r="T37" s="23"/>
+      <c r="Q37" s="19"/>
+      <c r="R37" s="40"/>
+      <c r="S37" s="40"/>
+      <c r="T37" s="41"/>
     </row>
     <row r="38" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B38" s="74"/>
-      <c r="C38" s="43" t="s">
-        <v>29</v>
-      </c>
-      <c r="D38" s="44"/>
-      <c r="E38" s="45"/>
+      <c r="B38" s="71"/>
+      <c r="C38" s="68" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" s="73"/>
+      <c r="E38" s="74"/>
       <c r="F38" s="23" t="s">
         <v>23</v>
       </c>
@@ -2262,19 +2276,19 @@
       <c r="M38" s="18"/>
       <c r="N38" s="18"/>
       <c r="O38" s="18"/>
-      <c r="P38" s="18"/>
+      <c r="P38" s="40"/>
       <c r="Q38" s="22"/>
       <c r="R38" s="22"/>
       <c r="S38" s="22"/>
       <c r="T38" s="23"/>
     </row>
     <row r="39" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B39" s="75"/>
-      <c r="C39" s="46"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="48"/>
+      <c r="B39" s="72"/>
+      <c r="C39" s="75"/>
+      <c r="D39" s="76"/>
+      <c r="E39" s="77"/>
       <c r="F39" s="23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G39" s="24"/>
       <c r="H39" s="22"/>
@@ -2285,21 +2299,21 @@
       <c r="M39" s="15"/>
       <c r="N39" s="15"/>
       <c r="O39" s="15"/>
-      <c r="P39" s="15"/>
+      <c r="P39" s="40"/>
       <c r="Q39" s="22"/>
       <c r="R39" s="22"/>
       <c r="S39" s="22"/>
       <c r="T39" s="23"/>
     </row>
     <row r="40" spans="2:20" ht="17.25" customHeight="1">
-      <c r="B40" s="50" t="s">
+      <c r="B40" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="51" t="s">
+      <c r="C40" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="D40" s="52"/>
-      <c r="E40" s="53"/>
+      <c r="D40" s="69"/>
+      <c r="E40" s="48"/>
       <c r="F40" s="23" t="s">
         <v>10</v>
       </c>
@@ -2319,12 +2333,12 @@
       <c r="T40" s="23"/>
     </row>
     <row r="41" spans="2:20" ht="17.25">
-      <c r="B41" s="50"/>
-      <c r="C41" s="51" t="s">
+      <c r="B41" s="51"/>
+      <c r="C41" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="D41" s="52"/>
-      <c r="E41" s="53"/>
+      <c r="D41" s="69"/>
+      <c r="E41" s="48"/>
       <c r="F41" s="23" t="s">
         <v>10</v>
       </c>
@@ -2344,12 +2358,12 @@
       <c r="T41" s="23"/>
     </row>
     <row r="42" spans="2:20" ht="17.25">
-      <c r="B42" s="50"/>
-      <c r="C42" s="51" t="s">
+      <c r="B42" s="51"/>
+      <c r="C42" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="D42" s="52"/>
-      <c r="E42" s="53"/>
+      <c r="D42" s="69"/>
+      <c r="E42" s="48"/>
       <c r="F42" s="23" t="s">
         <v>10</v>
       </c>
@@ -2369,12 +2383,12 @@
       <c r="T42" s="23"/>
     </row>
     <row r="43" spans="2:20" ht="18" thickBot="1">
-      <c r="B43" s="40" t="s">
+      <c r="B43" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="C43" s="41"/>
-      <c r="D43" s="41"/>
-      <c r="E43" s="42"/>
+      <c r="C43" s="66"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="67"/>
       <c r="F43" s="8" t="s">
         <v>15</v>
       </c>
@@ -2413,20 +2427,22 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="D23:D27"/>
-    <mergeCell ref="D18:D22"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="C18:C28"/>
-    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="B18:B39"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="C38:E39"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C30:C37"/>
+    <mergeCell ref="D30:E30"/>
     <mergeCell ref="D31:E31"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="B2:E3"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C6:E6"/>
@@ -2440,20 +2456,18 @@
     <mergeCell ref="C10:E11"/>
     <mergeCell ref="C12:E13"/>
     <mergeCell ref="C14:E15"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="C38:E39"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C32:C37"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="B18:B39"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B2:E3"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="O2:R2"/>
+    <mergeCell ref="D23:D27"/>
+    <mergeCell ref="D18:D22"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="C18:C27"/>
+    <mergeCell ref="C28:C29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>